<commit_message>
updateuserprofile no longer has null pointer upon page refresh. showuser now split into employer and candidate
</commit_message>
<xml_diff>
--- a/Vacit/UPLOAD_DIR/test.xlsx
+++ b/Vacit/UPLOAD_DIR/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Existentialism\Educom-Vacit\Vacit\UPLOAD_DIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E87640-9FBE-4512-AD8A-4FC055B6B1D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572A131F-224C-4B3A-9E6F-5B7A1751AB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{13319AB7-20EF-42E6-91B8-35F69CFE16E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>testpost</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>user_cv</t>
-  </si>
-  <si>
-    <t>testpass</t>
   </si>
   <si>
     <t>testpic</t>
@@ -464,7 +461,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,89 +513,89 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
       <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
       </c>
       <c r="J3" t="s">
         <v>0</v>
       </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
extra pictures for readme
</commit_message>
<xml_diff>
--- a/Vacit/UPLOAD_DIR/test.xlsx
+++ b/Vacit/UPLOAD_DIR/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Existentialism\Educom-Vacit\Vacit\UPLOAD_DIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D0E176-E99C-4283-836F-E9DE23994387}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1056378D-821C-45F9-821B-301A5FC370E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{13319AB7-20EF-42E6-91B8-35F69CFE16E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>username</t>
   </si>
@@ -66,28 +66,22 @@
     <t>user_cv</t>
   </si>
   <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Facebook</t>
-  </si>
-  <si>
-    <t>Uber</t>
-  </si>
-  <si>
-    <t>Educom</t>
-  </si>
-  <si>
-    <t>Microsoft</t>
-  </si>
-  <si>
-    <t>Tencent</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>Lenovo</t>
+    <t>AliBaba</t>
+  </si>
+  <si>
+    <t>DetaCom</t>
+  </si>
+  <si>
+    <t>Alphabet</t>
+  </si>
+  <si>
+    <t>Gameboy</t>
+  </si>
+  <si>
+    <t>Riot</t>
+  </si>
+  <si>
+    <t>Steam</t>
   </si>
 </sst>
 </file>
@@ -440,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8040EB05-8864-4239-AE73-FA669EA85D7F}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,22 +535,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>